<commit_message>
List resistors that should be checked
</commit_message>
<xml_diff>
--- a/test-leds.xlsx
+++ b/test-leds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_RevolutionRobotics\ProductionTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_RevolutionRobotics\Misc\ProductionTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3E775A-B172-4775-8E51-B91DC00B2640}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A0B64C-C10D-4841-AE3C-892E9FB956C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6831E35D-5F26-4C81-8723-278DA3AC94D5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="135">
   <si>
     <t>S1</t>
   </si>
@@ -79,6 +79,363 @@
   </si>
   <si>
     <t>IMU (accelerometer and gyroscope)</t>
+  </si>
+  <si>
+    <t>LED RED</t>
+  </si>
+  <si>
+    <t>Resistors to check</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>R120</t>
+  </si>
+  <si>
+    <t>47k</t>
+  </si>
+  <si>
+    <t>R147</t>
+  </si>
+  <si>
+    <t>R97</t>
+  </si>
+  <si>
+    <t>R102</t>
+  </si>
+  <si>
+    <t>R90</t>
+  </si>
+  <si>
+    <t>R91</t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>240k</t>
+  </si>
+  <si>
+    <t>R151</t>
+  </si>
+  <si>
+    <t>R154</t>
+  </si>
+  <si>
+    <t>R155</t>
+  </si>
+  <si>
+    <t>R159</t>
+  </si>
+  <si>
+    <t>R123</t>
+  </si>
+  <si>
+    <t>R125</t>
+  </si>
+  <si>
+    <t>R126</t>
+  </si>
+  <si>
+    <t>R129</t>
+  </si>
+  <si>
+    <t>R133</t>
+  </si>
+  <si>
+    <t>R135</t>
+  </si>
+  <si>
+    <t>R136</t>
+  </si>
+  <si>
+    <t>R138</t>
+  </si>
+  <si>
+    <t>R142</t>
+  </si>
+  <si>
+    <t>R145</t>
+  </si>
+  <si>
+    <t>R146</t>
+  </si>
+  <si>
+    <t>R152</t>
+  </si>
+  <si>
+    <t>R160</t>
+  </si>
+  <si>
+    <t>R124</t>
+  </si>
+  <si>
+    <t>R130</t>
+  </si>
+  <si>
+    <t>R134</t>
+  </si>
+  <si>
+    <t>R140</t>
+  </si>
+  <si>
+    <t>R143</t>
+  </si>
+  <si>
+    <t>R149</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>R63</t>
+  </si>
+  <si>
+    <t>R75</t>
+  </si>
+  <si>
+    <t>R58</t>
+  </si>
+  <si>
+    <t>R70</t>
+  </si>
+  <si>
+    <t>R78</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t>R66</t>
+  </si>
+  <si>
+    <t>R67</t>
+  </si>
+  <si>
+    <t>R79</t>
+  </si>
+  <si>
+    <t>R80</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>R46</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
+  <si>
+    <t>R60</t>
+  </si>
+  <si>
+    <t>R73</t>
+  </si>
+  <si>
+    <t>R74</t>
+  </si>
+  <si>
+    <t>R87</t>
+  </si>
+  <si>
+    <t>R88</t>
+  </si>
+  <si>
+    <t>39k</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R105</t>
+  </si>
+  <si>
+    <t>R107</t>
+  </si>
+  <si>
+    <t>R106</t>
+  </si>
+  <si>
+    <t>R108</t>
+  </si>
+  <si>
+    <t>R164</t>
+  </si>
+  <si>
+    <t>150k</t>
+  </si>
+  <si>
+    <t>R163</t>
+  </si>
+  <si>
+    <t>R157</t>
+  </si>
+  <si>
+    <t>R181</t>
+  </si>
+  <si>
+    <t>R137</t>
+  </si>
+  <si>
+    <t>R128</t>
+  </si>
+  <si>
+    <t>R158</t>
+  </si>
+  <si>
+    <t>R161</t>
+  </si>
+  <si>
+    <t>R156</t>
+  </si>
+  <si>
+    <t>R153</t>
+  </si>
+  <si>
+    <t>R150</t>
+  </si>
+  <si>
+    <t>R144</t>
+  </si>
+  <si>
+    <t>R141</t>
+  </si>
+  <si>
+    <t>R139</t>
+  </si>
+  <si>
+    <t>R132</t>
+  </si>
+  <si>
+    <t>R131</t>
+  </si>
+  <si>
+    <t>R127</t>
+  </si>
+  <si>
+    <t>R122</t>
+  </si>
+  <si>
+    <t>R121</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>R53</t>
+  </si>
+  <si>
+    <t>0.120</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R72</t>
+  </si>
+  <si>
+    <t>R77</t>
+  </si>
+  <si>
+    <t>R81</t>
+  </si>
+  <si>
+    <t>R82</t>
+  </si>
+  <si>
+    <t>R61</t>
+  </si>
+  <si>
+    <t>R64</t>
+  </si>
+  <si>
+    <t>R48</t>
+  </si>
+  <si>
+    <t>R55</t>
+  </si>
+  <si>
+    <t>R54</t>
+  </si>
+  <si>
+    <t>R84</t>
   </si>
 </sst>
 </file>
@@ -102,15 +459,45 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -118,13 +505,235 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -441,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405C6479-6E61-4F58-94DC-C62A924BF4E6}">
-  <dimension ref="B2:R13"/>
+  <dimension ref="B2:W111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="V100" sqref="V100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,9 +1066,11 @@
     <col min="8" max="8" width="13.42578125" hidden="1" customWidth="1"/>
     <col min="9" max="11" width="9.140625" hidden="1" customWidth="1"/>
     <col min="12" max="18" width="3.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -475,8 +1086,17 @@
       <c r="O2">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>2</v>
       </c>
@@ -495,8 +1115,17 @@
       <c r="P3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U3" s="5">
+        <v>1</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="W3" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -515,8 +1144,15 @@
       <c r="Q4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U4" s="6"/>
+      <c r="V4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="W4" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>4</v>
       </c>
@@ -535,8 +1171,15 @@
       <c r="R5">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U5" s="6"/>
+      <c r="V5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="W5" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E6" s="1">
         <v>9</v>
       </c>
@@ -549,8 +1192,15 @@
       <c r="Q6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U6" s="6"/>
+      <c r="V6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="W6" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E7" s="1">
         <v>10</v>
       </c>
@@ -563,8 +1213,15 @@
       <c r="P7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U7" s="6"/>
+      <c r="V7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="W7" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E8" s="1">
         <v>11</v>
       </c>
@@ -574,16 +1231,30 @@
       <c r="O8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U8" s="6"/>
+      <c r="V8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="W8" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E9" s="1">
         <v>12</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U9" s="6"/>
+      <c r="V9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="W9" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E10" s="1">
         <v>13</v>
       </c>
@@ -602,29 +1273,967 @@
       <c r="Q10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U10" s="6"/>
+      <c r="V10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W10" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E11" s="1">
         <v>14</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U11" s="6"/>
+      <c r="V11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="W11" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E12" s="1">
         <v>15</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U12" s="6"/>
+      <c r="V12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="W12" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
         <v>16</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>
+      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="W13" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U14" s="6"/>
+      <c r="V14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="W14" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U15" s="6"/>
+      <c r="V15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="W15" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U16" s="6"/>
+      <c r="V16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="W16" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U17" s="6"/>
+      <c r="V17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="W17" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U18" s="6"/>
+      <c r="V18" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="W18" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U19" s="6"/>
+      <c r="V19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="W19" s="24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U20" s="6"/>
+      <c r="V20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="W20" s="25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="21" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U21" s="6"/>
+      <c r="V21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="W21" s="25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="22" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U22" s="6"/>
+      <c r="V22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W22" s="25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="23" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U23" s="6"/>
+      <c r="V23" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="W23" s="26">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="24" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U24" s="6"/>
+      <c r="V24" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="W24" s="27">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="25" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U25" s="6"/>
+      <c r="V25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="W25" s="27">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="26" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U26" s="6"/>
+      <c r="V26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="W26" s="27">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="27" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U27" s="6"/>
+      <c r="V27" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="W27" s="28">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="28" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U28" s="6"/>
+      <c r="V28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="W28" s="25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="29" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U29" s="6"/>
+      <c r="V29" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="W29" s="25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="30" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U30" s="6"/>
+      <c r="V30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="W30" s="25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="31" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U31" s="6"/>
+      <c r="V31" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="W31" s="25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="32" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U32" s="6"/>
+      <c r="V32" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="W32" s="25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="33" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U33" s="6"/>
+      <c r="V33" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="W33" s="26">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="34" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U34" s="6"/>
+      <c r="V34" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="W34" s="27">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="35" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U35" s="6"/>
+      <c r="V35" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="W35" s="27">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="36" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U36" s="6"/>
+      <c r="V36" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="W36" s="27">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="37" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U37" s="6"/>
+      <c r="V37" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="W37" s="27">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="38" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U38" s="6"/>
+      <c r="V38" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="W38" s="27">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="39" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U39" s="6"/>
+      <c r="V39" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="W39" s="28">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="40" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U40" s="6"/>
+      <c r="V40" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="W40" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U41" s="6"/>
+      <c r="V41" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="W41" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U42" s="6"/>
+      <c r="V42" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="W42" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U43" s="6"/>
+      <c r="V43" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="W43" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U44" s="6"/>
+      <c r="V44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="W44" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U45" s="6"/>
+      <c r="V45" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="W45" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U46" s="6"/>
+      <c r="V46" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="W46" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U47" s="6"/>
+      <c r="V47" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W47" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U48" s="6"/>
+      <c r="V48" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W48" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U49" s="6"/>
+      <c r="V49" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="W49" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U50" s="6"/>
+      <c r="V50" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="W50" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U51" s="6"/>
+      <c r="V51" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="W51" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U52" s="6"/>
+      <c r="V52" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="W52" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U53" s="6"/>
+      <c r="V53" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="W53" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U54" s="6"/>
+      <c r="V54" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="W54" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U55" s="6"/>
+      <c r="V55" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="W55" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U56" s="6"/>
+      <c r="V56" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="W56" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U57" s="6"/>
+      <c r="V57" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="W57" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U58" s="6"/>
+      <c r="V58" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="W58" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U59" s="6"/>
+      <c r="V59" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="W59" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U60" s="6"/>
+      <c r="V60" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="W60" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U61" s="6"/>
+      <c r="V61" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="W61" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U62" s="6"/>
+      <c r="V62" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="W62" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U63" s="12"/>
+      <c r="V63" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="W63" s="32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U64" s="20">
+        <v>2</v>
+      </c>
+      <c r="V64" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="W64" s="33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U65" s="19"/>
+      <c r="V65" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="W65" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U66" s="19"/>
+      <c r="V66" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="W66" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U67" s="19"/>
+      <c r="V67" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="W67" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U68" s="21"/>
+      <c r="V68" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="W68" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U69" s="20">
+        <v>3</v>
+      </c>
+      <c r="V69" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="W69" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U70" s="6"/>
+      <c r="V70" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="W70" s="34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U71" s="6"/>
+      <c r="V71" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="W71" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U72" s="6"/>
+      <c r="V72" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="W72" s="36">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="73" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U73" s="12"/>
+      <c r="V73" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="W73" s="37">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="74" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U74" s="20">
+        <v>4</v>
+      </c>
+      <c r="V74" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="W74" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U75" s="6"/>
+      <c r="V75" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="W75" s="34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="76" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U76" s="6"/>
+      <c r="V76" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="W76" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U77" s="6"/>
+      <c r="V77" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="W77" s="36">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="78" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U78" s="12"/>
+      <c r="V78" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="W78" s="37">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="79" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U79" s="20">
+        <v>5</v>
+      </c>
+      <c r="V79" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="W79" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U80" s="6"/>
+      <c r="V80" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="W80" s="34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="81" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U81" s="6"/>
+      <c r="V81" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="W81" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U82" s="6"/>
+      <c r="V82" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="W82" s="36">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="83" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U83" s="12"/>
+      <c r="V83" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="W83" s="37">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="84" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U84" s="20">
+        <v>6</v>
+      </c>
+      <c r="V84" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="W84" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U85" s="6"/>
+      <c r="V85" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="W85" s="34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="86" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U86" s="6"/>
+      <c r="V86" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="W86" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U87" s="6"/>
+      <c r="V87" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="W87" s="36">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="88" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U88" s="12"/>
+      <c r="V88" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="W88" s="37">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="89" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U89" s="2">
+        <v>7</v>
+      </c>
+      <c r="V89" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="W89" s="38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U90" s="3"/>
+      <c r="V90" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="W90" s="39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U91" s="4"/>
+      <c r="V91" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="W91" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="92" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U92" s="2">
+        <v>8</v>
+      </c>
+      <c r="V92" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="W92" s="38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U93" s="3"/>
+      <c r="V93" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="W93" s="39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="94" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U94" s="4"/>
+      <c r="V94" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="W94" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="95" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U95" s="2">
+        <v>9</v>
+      </c>
+      <c r="V95" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="W95" s="38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U96" s="3"/>
+      <c r="V96" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="W96" s="39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U97" s="4"/>
+      <c r="V97" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="W97" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="98" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U98" s="2">
+        <v>10</v>
+      </c>
+      <c r="V98" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="W98" s="38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U99" s="3"/>
+      <c r="V99" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="W99" s="39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U100" s="4"/>
+      <c r="V100" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="W100" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="101" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U101" s="2">
+        <v>11</v>
+      </c>
+      <c r="V101" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="W101" s="38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U102" s="3"/>
+      <c r="V102" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="W102" s="39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U103" s="4"/>
+      <c r="V103" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="W103" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="104" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U104" s="2">
+        <v>12</v>
+      </c>
+      <c r="V104" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="W104" s="38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U105" s="3"/>
+      <c r="V105" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="W105" s="39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U106" s="4"/>
+      <c r="V106" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="W106" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="107" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U107" s="41">
+        <v>13</v>
+      </c>
+      <c r="V107" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="W107" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="108" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U108" s="2">
+        <v>14</v>
+      </c>
+      <c r="V108" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="W108" s="38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="109" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U109" s="4"/>
+      <c r="V109" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="W109" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="110" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U110" s="2">
+        <v>15</v>
+      </c>
+      <c r="V110" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="W110" s="38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="111" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U111" s="4"/>
+      <c r="V111" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="W111" s="40" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>